<commit_message>
Update Foot Pedal main functions
Now triggers tension
</commit_message>
<xml_diff>
--- a/Foot Controller/FootPedalInfo_Excel.xlsx
+++ b/Foot Controller/FootPedalInfo_Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aspit\Git\PerforM4L\Foot Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E21AB4-C757-438F-AA80-6E0370D8283E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF603D1A-886C-4E6B-B061-F48681C11C9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8688" yWindow="1080" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JSON-CSV.COM results" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="52">
   <si>
     <t>Row 0</t>
   </si>
@@ -34,12 +34,6 @@
     <t>Next Scene</t>
   </si>
   <si>
-    <t>Unarm All Tracks</t>
-  </si>
-  <si>
-    <t>Arm Selected Track</t>
-  </si>
-  <si>
     <t>Stop Armed Track</t>
   </si>
   <si>
@@ -91,36 +85,9 @@
     <t>Row 2</t>
   </si>
   <si>
-    <t>Bypass (Chord Player)</t>
-  </si>
-  <si>
-    <t>Flush</t>
-  </si>
-  <si>
-    <t>Legato</t>
-  </si>
-  <si>
-    <t>Midilearn</t>
-  </si>
-  <si>
-    <t>Keylearn</t>
-  </si>
-  <si>
-    <t>Learn</t>
-  </si>
-  <si>
-    <t>Clear</t>
-  </si>
-  <si>
-    <t>Clearall</t>
-  </si>
-  <si>
     <t>Nothing</t>
   </si>
   <si>
-    <t>Reread Chords</t>
-  </si>
-  <si>
     <t>Row 3</t>
   </si>
   <si>
@@ -139,33 +106,6 @@
     <t>Row 4</t>
   </si>
   <si>
-    <t>Glove Serial On</t>
-  </si>
-  <si>
-    <t>Glove Serial Off</t>
-  </si>
-  <si>
-    <t>Map X</t>
-  </si>
-  <si>
-    <t>Map Y</t>
-  </si>
-  <si>
-    <t>Map Z</t>
-  </si>
-  <si>
-    <t>Half Mode</t>
-  </si>
-  <si>
-    <t>Unmap X</t>
-  </si>
-  <si>
-    <t>Unmap Y</t>
-  </si>
-  <si>
-    <t>Unmap Z</t>
-  </si>
-  <si>
     <t>Row 5</t>
   </si>
   <si>
@@ -206,6 +146,36 @@
   </si>
   <si>
     <t>Select Armed Tracks</t>
+  </si>
+  <si>
+    <t>Map Glove X</t>
+  </si>
+  <si>
+    <t>Map Glove Y</t>
+  </si>
+  <si>
+    <t>Map Glove Z</t>
+  </si>
+  <si>
+    <t>Unmap Glove X</t>
+  </si>
+  <si>
+    <t>Unmap Glove Y</t>
+  </si>
+  <si>
+    <t>Unmap Glove Z</t>
+  </si>
+  <si>
+    <t>Tension Start</t>
+  </si>
+  <si>
+    <t>Tension Cancel</t>
+  </si>
+  <si>
+    <t>Go To Tension</t>
+  </si>
+  <si>
+    <t>Disarm All Tracks</t>
   </si>
 </sst>
 </file>
@@ -221,7 +191,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -557,7 +526,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,19 +546,19 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -600,19 +569,19 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -623,19 +592,19 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -646,19 +615,19 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -666,22 +635,22 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -689,22 +658,22 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -712,22 +681,22 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -735,22 +704,22 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -758,22 +727,22 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -781,22 +750,22 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -804,36 +773,36 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -841,16 +810,16 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -858,16 +827,16 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -875,16 +844,16 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -892,16 +861,16 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -909,16 +878,16 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -926,16 +895,16 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -943,16 +912,16 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -960,16 +929,16 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -977,16 +946,16 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E24" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -994,16 +963,16 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>